<commit_message>
[Fix] SpriteManager / CharacterData / UICharacterRecipe 수정
</commit_message>
<xml_diff>
--- a/character_data.xlsx
+++ b/character_data.xlsx
@@ -5,11 +5,11 @@
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krsoft\OneDrive\Desktop\Random Combination Defence - Great Man\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FORYOUCOM\Desktop\Defence Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="28545" windowHeight="11460"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="17715" windowHeight="6330"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -42,96 +42,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <x:si>
     <x:t>테스트 스킬 3</x:t>
   </x:si>
   <x:si>
+    <x:t>move_speed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>테스트 스킬 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유일한</x:t>
+  </x:si>
+  <x:si>
+    <x:t>int</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽</x:t>
+  </x:si>
+  <x:si>
     <x:t>안흔한</x:t>
   </x:si>
   <x:si>
-    <x:t>주몽</x:t>
-  </x:si>
-  <x:si>
     <x:t>이순신</x:t>
   </x:si>
   <x:si>
-    <x:t>유일한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>int</x:t>
+    <x:t>흔한</x:t>
   </x:si>
   <x:si>
     <x:t>희귀한</x:t>
   </x:si>
   <x:si>
-    <x:t>흔한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>image/character/이순신</x:t>
-  </x:si>
-  <x:si>
-    <x:t>image/character/안흔한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>image/character/희귀한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>image/character/유일한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>image/character/흔한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>image/character/주몽</x:t>
-  </x:si>
-  <x:si>
-    <x:t>move_speed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>테스트 스킬 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>character_image_path</x:t>
+    <x:t>attack_range</x:t>
+  </x:si>
+  <x:si>
+    <x:t>attack_speed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>skill_3_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>skill_2_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>skill_1_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>string</x:t>
+  </x:si>
+  <x:si>
+    <x:t>damage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>float</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화살 날리기</x:t>
   </x:si>
   <x:si>
     <x:t>tier</x:t>
   </x:si>
   <x:si>
-    <x:t>화살 날리기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>float</x:t>
+    <x:t>name</x:t>
   </x:si>
   <x:si>
     <x:t>테스트 스킬</x:t>
   </x:si>
   <x:si>
-    <x:t>string</x:t>
-  </x:si>
-  <x:si>
     <x:t>불화살 날리기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>damage</x:t>
-  </x:si>
-  <x:si>
-    <x:t>attack_range</x:t>
-  </x:si>
-  <x:si>
-    <x:t>skill_3_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>skill_2_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>attack_speed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>skill_1_name</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -230,7 +209,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="5">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -273,6 +252,9 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -576,7 +558,7 @@
   <x:dimension ref="A1:J8"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="J15" activeCellId="0" sqref="J15:J15"/>
+      <x:selection activeCell="J10" activeCellId="0" sqref="J10:J10"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
@@ -601,71 +583,67 @@
   <x:sheetData>
     <x:row r="1" spans="1:10">
       <x:c r="A1" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>28</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E1" s="1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="G1" s="1" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="F1" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="G1" s="1" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="H1" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="I1" s="1" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="J1" s="1" t="s">
-        <x:v>16</x:v>
-      </x:c>
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="J1" s="4"/>
     </x:row>
     <x:row r="2" spans="1:10">
       <x:c r="A2" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="D2" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="E2" s="2" t="s">
-        <x:v>19</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="F2" s="2" t="s">
-        <x:v>5</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="G2" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="H2" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="I2" s="2" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="J2" s="2" t="s">
-        <x:v>21</x:v>
-      </x:c>
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="J2" s="4"/>
     </x:row>
     <x:row r="3" spans="1:10">
       <x:c r="A3" s="3" t="s">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B3" s="3">
         <x:v>20</x:v>
@@ -689,13 +667,11 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="I3" s="3"/>
-      <x:c r="J3" s="3" t="s">
-        <x:v>13</x:v>
-      </x:c>
+      <x:c r="J3" s="4"/>
     </x:row>
     <x:row r="4" spans="1:10">
       <x:c r="A4" s="3" t="s">
-        <x:v>3</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B4" s="3">
         <x:v>15</x:v>
@@ -715,13 +691,11 @@
       <x:c r="G4" s="3"/>
       <x:c r="H4" s="3"/>
       <x:c r="I4" s="3"/>
-      <x:c r="J4" s="3" t="s">
-        <x:v>8</x:v>
-      </x:c>
+      <x:c r="J4" s="4"/>
     </x:row>
     <x:row r="5" spans="1:10">
       <x:c r="A5" s="3" t="s">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B5" s="3">
         <x:v>10</x:v>
@@ -741,13 +715,11 @@
       <x:c r="G5" s="3"/>
       <x:c r="H5" s="3"/>
       <x:c r="I5" s="3"/>
-      <x:c r="J5" s="3" t="s">
-        <x:v>11</x:v>
-      </x:c>
+      <x:c r="J5" s="4"/>
     </x:row>
     <x:row r="6" spans="1:10">
       <x:c r="A6" s="3" t="s">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B6" s="3">
         <x:v>5</x:v>
@@ -767,13 +739,11 @@
       <x:c r="G6" s="3"/>
       <x:c r="H6" s="3"/>
       <x:c r="I6" s="3"/>
-      <x:c r="J6" s="3" t="s">
-        <x:v>10</x:v>
-      </x:c>
+      <x:c r="J6" s="4"/>
     </x:row>
     <x:row r="7" spans="1:10">
       <x:c r="A7" s="3" t="s">
-        <x:v>1</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B7" s="3">
         <x:v>3</x:v>
@@ -793,13 +763,11 @@
       <x:c r="G7" s="3"/>
       <x:c r="H7" s="3"/>
       <x:c r="I7" s="3"/>
-      <x:c r="J7" s="3" t="s">
-        <x:v>9</x:v>
-      </x:c>
+      <x:c r="J7" s="4"/>
     </x:row>
     <x:row r="8" spans="1:10">
       <x:c r="A8" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B8" s="3">
         <x:v>1</x:v>
@@ -817,17 +785,15 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="G8" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H8" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="I8" s="3" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="J8" s="3" t="s">
-        <x:v>12</x:v>
-      </x:c>
+      <x:c r="J8" s="4"/>
     </x:row>
   </x:sheetData>
   <x:pageMargins left="0.69972223043441772461" right="0.69972223043441772461" top="0.75" bottom="0.75" header="0.30000001192092895508" footer="0.30000001192092895508"/>

</xml_diff>

<commit_message>
[Refactor] 변수명 통일 중 - tier를 tierNum(정수), tierName(문자열), itemClass(서버)로 통일
</commit_message>
<xml_diff>
--- a/character_data.xlsx
+++ b/character_data.xlsx
@@ -5,11 +5,11 @@
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krsoft\OneDrive\Desktop\Random Combination Defence - Great Man\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FORYOUCOM\Desktop\Defence Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="6780"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="17715" windowHeight="6330"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -44,19 +44,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <x:si>
+    <x:t>테스트 스킬 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>테스트 스킬 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>move_speed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>skill_3_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>skill_1_name</x:t>
+  </x:si>
+  <x:si>
     <x:t>display_name</x:t>
   </x:si>
   <x:si>
+    <x:t>skill_2_name</x:t>
+  </x:si>
+  <x:si>
+    <x:t>attack_speed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>attack_range</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화살 날리기</x:t>
+  </x:si>
+  <x:si>
     <x:t>string</x:t>
   </x:si>
   <x:si>
     <x:t>float</x:t>
   </x:si>
   <x:si>
-    <x:t>tier</x:t>
-  </x:si>
-  <x:si>
-    <x:t>화살 날리기</x:t>
+    <x:t>불화살 날리기</x:t>
   </x:si>
   <x:si>
     <x:t>테스트 스킬</x:t>
@@ -65,52 +89,28 @@
     <x:t>damage</x:t>
   </x:si>
   <x:si>
-    <x:t>불화살 날리기</x:t>
-  </x:si>
-  <x:si>
-    <x:t>테스트 스킬 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>move_speed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>테스트 스킬 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>attack_range</x:t>
-  </x:si>
-  <x:si>
-    <x:t>attack_speed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>skill_3_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>skill_2_name</x:t>
-  </x:si>
-  <x:si>
-    <x:t>skill_1_name</x:t>
-  </x:si>
-  <x:si>
     <x:t>흔한</x:t>
   </x:si>
   <x:si>
+    <x:t>안흔한</x:t>
+  </x:si>
+  <x:si>
+    <x:t>주몽</x:t>
+  </x:si>
+  <x:si>
+    <x:t>유일한</x:t>
+  </x:si>
+  <x:si>
+    <x:t>희귀한</x:t>
+  </x:si>
+  <x:si>
+    <x:t>int</x:t>
+  </x:si>
+  <x:si>
     <x:t>이순신</x:t>
   </x:si>
   <x:si>
-    <x:t>유일한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>안흔한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>주몽</x:t>
-  </x:si>
-  <x:si>
-    <x:t>희귀한</x:t>
-  </x:si>
-  <x:si>
-    <x:t>int</x:t>
+    <x:t>tier_num</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -558,7 +558,7 @@
   <x:dimension ref="A1:J8"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="D11" activeCellId="0" sqref="D11:D11"/>
+      <x:selection activeCell="H11" activeCellId="0" sqref="H11:H11"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
@@ -568,7 +568,7 @@
     <x:col min="3" max="3" width="12.0234375" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="11.89453125" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="11.51171875" bestFit="1" customWidth="1"/>
-    <x:col min="6" max="6" width="3.796875" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="6" width="8.4765625" bestFit="1" customWidth="1"/>
     <x:col min="7" max="7" width="11.640625" bestFit="1" customWidth="1"/>
     <x:col min="8" max="8" width="13.03125" bestFit="1" customWidth="1"/>
     <x:col min="9" max="9" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -583,67 +583,67 @@
   <x:sheetData>
     <x:row r="1" spans="1:10">
       <x:c r="A1" s="1" t="s">
-        <x:v>0</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E1" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F1" s="1" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="G1" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="H1" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="C1" s="1" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D1" s="1" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="E1" s="1" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F1" s="1" t="s">
+      <x:c r="I1" s="1" t="s">
         <x:v>3</x:v>
-      </x:c>
-      <x:c r="G1" s="1" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="H1" s="1" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="I1" s="1" t="s">
-        <x:v>13</x:v>
       </x:c>
       <x:c r="J1" s="4"/>
     </x:row>
     <x:row r="2" spans="1:10">
       <x:c r="A2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="B2" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="D2" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="E2" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="F2" s="2" t="s">
-        <x:v>22</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="G2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="H2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="I2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="J2" s="4"/>
     </x:row>
     <x:row r="3" spans="1:10">
       <x:c r="A3" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B3" s="3">
         <x:v>20</x:v>
@@ -661,17 +661,17 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="G3" s="3" t="s">
-        <x:v>4</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="H3" s="3" t="s">
-        <x:v>7</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="I3" s="3"/>
       <x:c r="J3" s="4"/>
     </x:row>
     <x:row r="4" spans="1:10">
       <x:c r="A4" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B4" s="3">
         <x:v>15</x:v>
@@ -719,7 +719,7 @@
     </x:row>
     <x:row r="6" spans="1:10">
       <x:c r="A6" s="3" t="s">
-        <x:v>21</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B6" s="3">
         <x:v>5</x:v>
@@ -743,7 +743,7 @@
     </x:row>
     <x:row r="7" spans="1:10">
       <x:c r="A7" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B7" s="3">
         <x:v>3</x:v>
@@ -767,7 +767,7 @@
     </x:row>
     <x:row r="8" spans="1:10">
       <x:c r="A8" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B8" s="3">
         <x:v>1</x:v>
@@ -785,13 +785,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="G8" s="3" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="H8" s="3" t="s">
-        <x:v>8</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I8" s="3" t="s">
-        <x:v>10</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="J8" s="4"/>
     </x:row>

</xml_diff>